<commit_message>
Added a few hats (currently broken))
</commit_message>
<xml_diff>
--- a/Hats Spreadsheet V2.xlsx
+++ b/Hats Spreadsheet V2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s4101141\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Github repos\ExperimentalGames\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40CB1FB5-96AA-47AF-9E4E-5AD33E960BF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5305A48A-2536-4E5A-B003-AF86D22E009B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{3EB3C7D8-FC78-4C7F-BA3B-069845290569}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3EB3C7D8-FC78-4C7F-BA3B-069845290569}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -767,8 +767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B7122BC-1FA8-4F8A-8E88-D6846949F0A0}">
   <dimension ref="A1:E102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="F77" sqref="F77"/>
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="B102" sqref="B102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1063,7 +1063,7 @@
         <v>35</v>
       </c>
       <c r="E33" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1566,7 +1566,7 @@
         <v>103</v>
       </c>
       <c r="E94" t="s">
-        <v>111</v>
+        <v>83</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -1598,6 +1598,7 @@
       <c r="A98" t="s">
         <v>107</v>
       </c>
+      <c r="B98" s="2"/>
       <c r="E98" t="s">
         <v>81</v>
       </c>
@@ -1606,6 +1607,7 @@
       <c r="A99" t="s">
         <v>108</v>
       </c>
+      <c r="B99" s="2"/>
       <c r="E99" t="s">
         <v>81</v>
       </c>
@@ -1614,6 +1616,7 @@
       <c r="A100" t="s">
         <v>109</v>
       </c>
+      <c r="B100" s="2"/>
       <c r="E100" t="s">
         <v>81</v>
       </c>

</xml_diff>